<commit_message>
Uploading excel with initial values.
</commit_message>
<xml_diff>
--- a/src/main/java/com/neu/psa/tic/tac/toe/game/ExcelUtils/data.xlsx
+++ b/src/main/java/com/neu/psa/tic/tac/toe/game/ExcelUtils/data.xlsx
@@ -2,12 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <bookViews>
-    <workbookView activeTab="0"/>
-  </bookViews>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
+  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
@@ -61,7 +59,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -307,7 +304,6 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -347,12 +343,30 @@
         <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>100.0</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.0</v>
       </c>
       <c r="D2" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="J2" s="1">
         <v>0.0</v>
       </c>
     </row>
@@ -360,12 +374,63 @@
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B4" s="1">
+        <v>0.0</v>
+      </c>
       <c r="C4" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="J4" s="1">
         <v>0.0</v>
       </c>
     </row>
@@ -373,10 +438,64 @@
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B5" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
beta branch with bugs
</commit_message>
<xml_diff>
--- a/src/main/java/com/neu/psa/tic/tac/toe/game/ExcelUtils/data.xlsx
+++ b/src/main/java/com/neu/psa/tic/tac/toe/game/ExcelUtils/data.xlsx
@@ -2,10 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
@@ -59,6 +61,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -304,6 +307,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -342,31 +346,31 @@
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="B2" s="1" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J2" s="1" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -374,31 +378,31 @@
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="B3" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="1" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -406,31 +410,31 @@
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="B4" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J4" s="1" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -438,31 +442,31 @@
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="B5" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="1" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -470,31 +474,31 @@
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="B6" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>